<commit_message>
Added getName method in FileReader class and confirmed that the GUI can read from and subsequently display the name of the project on the UI
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -11,31 +11,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>This</t>
-  </si>
-  <si>
-    <t>Is</t>
-  </si>
-  <si>
-    <t>an</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example </t>
-  </si>
-  <si>
-    <t>spreadsheet</t>
-  </si>
-  <si>
-    <t>!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Pieces</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material </t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Total Material</t>
+  </si>
+  <si>
+    <t>Test Project!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -43,9 +46,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,12 +69,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -298,12 +317,24 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed FileWrite class so that it now writes data to the same sheet in excel. Added logic to keep track of the current blank cell number so each piece is saved in a new row. Greatly simplified FileReader class by changing position of project name in excel file.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -8,23 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A6422-7E9D-429B-93B3-D7C861CF3139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A747-00B2-44FE-879F-8905F40F7CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Project Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Pieces</t>
   </si>
@@ -41,7 +37,7 @@
     <t>Total Material</t>
   </si>
   <si>
-    <t>Test Project!</t>
+    <t>YAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -88,13 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -313,63 +306,50 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+    <row r="2">
+      <c r="D2" t="n" s="0">
+        <v>2.0</v>
+      </c>
     </row>
+    <row r="3">
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="2">
-      <c r="D2" t="n" s="0">
-        <v>43.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Continued to update FileWriter class. Confirmed that Material and time values from GUI can now save to excel file. Formatted Adapter, ModelFascade, FileWriter to be more clean. Added comments throughout.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D507A747-00B2-44FE-879F-8905F40F7CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A4015-D64E-4955-97F2-97A715EFB2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Pieces</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -37,14 +34,16 @@
     <t>Total Material</t>
   </si>
   <si>
-    <t>YAAAAAA</t>
+    <t>Project Name!</t>
+  </si>
+  <si>
+    <t>Piece #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -306,49 +305,88 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="D2" t="n" s="0">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="D3" t="n" s="0">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Successfully replaced giant if-else block in GUI with switch. Confirmed machine and code are working the same.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A4015-D64E-4955-97F2-97A715EFB2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1535853-7E6C-4C77-91B0-64B70E552DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added error message textfield and implemented for Angle, position and length violations on the GUI. Displays the error when the user makes it and change the color to red for 5 seconds.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
@@ -44,6 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -313,7 +314,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -338,52 +339,64 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="B2" s="0">
         <v>1</v>
       </c>
+      <c r="C2" t="n" s="0">
+        <v>1.2170000076293945</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>-1.0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="0">
         <v>2</v>
       </c>
+      <c r="C3" t="n" s="0">
+        <v>2.555999994277954</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>-1.0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="B6" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10">
+      <c r="B10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added and tested functionality of progress bar. Added more guardrails and warnings for bad user inputs on angle and position. Cleaned up useless Sytem.out.println statements.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -364,6 +364,12 @@
       <c r="B4" s="0">
         <v>3</v>
       </c>
+      <c r="C4" t="n" s="0">
+        <v>113.4229965209961</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>-1.0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="0">

</xml_diff>

<commit_message>
Made constants class to get rid of string values throughout code. Fixed bug with progress bar not resetting between pieces. Fixed bug with progress bar not calculating correctly after cuts.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -355,15 +355,33 @@
       <c r="B3" s="0">
         <v>2</v>
       </c>
+      <c r="C3" t="n" s="0">
+        <v>3.5799999237060547</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B4" s="0">
         <v>3</v>
       </c>
+      <c r="C4" t="n" s="0">
+        <v>36.4640007019043</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B5" s="0">
         <v>4</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>8.08899974822998</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>15.0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up a few more classes by removing unneeded println statements and added more constants to constants class.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD86C3FB-87D9-43DE-858C-77460C78AF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D03B18D-1FEA-459F-A710-7AD8AC064BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -309,14 +308,14 @@
   <dimension ref="A1:G404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.6640625"/>
-    <col min="6" max="6" customWidth="true" width="19.77734375"/>
-    <col min="7" max="7" customWidth="true" width="21.88671875"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -341,2041 +340,2017 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B2" s="0">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="n" s="0">
-        <v>9.878999710083008</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>3.0</v>
-      </c>
     </row>
     <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B3" s="0">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>3.5799999237060547</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>3.0</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B4" s="0">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>36.4640007019043</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>15.0</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B5" s="0">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="n" s="0">
-        <v>8.08899974822998</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>15.0</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B6" s="0">
+      <c r="B6">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B7" s="0">
+      <c r="B7">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="0">
+      <c r="B8">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="0">
+      <c r="B9">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="0">
+      <c r="B10">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="0">
+      <c r="B11">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="0">
+      <c r="B12">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="0">
+      <c r="B13">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="0">
+      <c r="B14">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="0">
+      <c r="B15">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="0">
+      <c r="B16">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="0">
+      <c r="B17">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="0">
+      <c r="B18">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="0">
+      <c r="B19">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="0">
+      <c r="B20">
         <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="0">
+      <c r="B21">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="0">
+      <c r="B22">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="0">
+      <c r="B23">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="0">
+      <c r="B24">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="0">
+      <c r="B25">
         <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="0">
+      <c r="B26">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="0">
+      <c r="B27">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="0">
+      <c r="B28">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="0">
+      <c r="B29">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="0">
+      <c r="B30">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="0">
+      <c r="B31">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="0">
+      <c r="B32">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="0">
+      <c r="B33">
         <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="0">
+      <c r="B34">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="0">
+      <c r="B35">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="0">
+      <c r="B36">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="0">
+      <c r="B37">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="0">
+      <c r="B38">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="0">
+      <c r="B39">
         <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="0">
+      <c r="B40">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="0">
+      <c r="B41">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="0">
+      <c r="B42">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="0">
+      <c r="B43">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="0">
+      <c r="B44">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="0">
+      <c r="B45">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="0">
+      <c r="B46">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="0">
+      <c r="B47">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="0">
+      <c r="B48">
         <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="0">
+      <c r="B49">
         <v>48</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="0">
+      <c r="B50">
         <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="0">
+      <c r="B51">
         <v>50</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="0">
+      <c r="B52">
         <v>51</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="0">
+      <c r="B53">
         <v>52</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="0">
+      <c r="B54">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="0">
+      <c r="B55">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="0">
+      <c r="B56">
         <v>55</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="0">
+      <c r="B57">
         <v>56</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="0">
+      <c r="B58">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="0">
+      <c r="B59">
         <v>58</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="0">
+      <c r="B60">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="0">
+      <c r="B61">
         <v>60</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="0">
+      <c r="B62">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="0">
+      <c r="B63">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="0">
+      <c r="B64">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="0">
+      <c r="B65">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="0">
+      <c r="B66">
         <v>65</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="0">
+      <c r="B67">
         <v>66</v>
       </c>
     </row>
     <row r="68" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="0">
+      <c r="B68">
         <v>67</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="0">
+      <c r="B69">
         <v>68</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="0">
+      <c r="B70">
         <v>69</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="0">
+      <c r="B71">
         <v>70</v>
       </c>
     </row>
     <row r="72" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="0">
+      <c r="B72">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="0">
+      <c r="B73">
         <v>72</v>
       </c>
     </row>
     <row r="74" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="0">
+      <c r="B74">
         <v>73</v>
       </c>
     </row>
     <row r="75" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="0">
+      <c r="B75">
         <v>74</v>
       </c>
     </row>
     <row r="76" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="0">
+      <c r="B76">
         <v>75</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="0">
+      <c r="B77">
         <v>76</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="0">
+      <c r="B78">
         <v>77</v>
       </c>
     </row>
     <row r="79" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="0">
+      <c r="B79">
         <v>78</v>
       </c>
     </row>
     <row r="80" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="0">
+      <c r="B80">
         <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="0">
+      <c r="B81">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="0">
+      <c r="B82">
         <v>81</v>
       </c>
     </row>
     <row r="83" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="0">
+      <c r="B83">
         <v>82</v>
       </c>
     </row>
     <row r="84" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="0">
+      <c r="B84">
         <v>83</v>
       </c>
     </row>
     <row r="85" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="0">
+      <c r="B85">
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="0">
+      <c r="B86">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="0">
+      <c r="B87">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="0">
+      <c r="B88">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="0">
+      <c r="B89">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="0">
+      <c r="B90">
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="0">
+      <c r="B91">
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="0">
+      <c r="B92">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="0">
+      <c r="B93">
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="0">
+      <c r="B94">
         <v>93</v>
       </c>
     </row>
     <row r="95" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="0">
+      <c r="B95">
         <v>94</v>
       </c>
     </row>
     <row r="96" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="0">
+      <c r="B96">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="0">
+      <c r="B97">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="0">
+      <c r="B98">
         <v>97</v>
       </c>
     </row>
     <row r="99" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="0">
+      <c r="B99">
         <v>98</v>
       </c>
     </row>
     <row r="100" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="0">
+      <c r="B100">
         <v>99</v>
       </c>
     </row>
     <row r="101" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="0">
+      <c r="B101">
         <v>100</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="0">
+      <c r="B102">
         <v>101</v>
       </c>
     </row>
     <row r="103" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="0">
+      <c r="B103">
         <v>102</v>
       </c>
     </row>
     <row r="104" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="0">
+      <c r="B104">
         <v>103</v>
       </c>
     </row>
     <row r="105" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="0">
+      <c r="B105">
         <v>104</v>
       </c>
     </row>
     <row r="106" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="0">
+      <c r="B106">
         <v>105</v>
       </c>
     </row>
     <row r="107" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="0">
+      <c r="B107">
         <v>106</v>
       </c>
     </row>
     <row r="108" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="0">
+      <c r="B108">
         <v>107</v>
       </c>
     </row>
     <row r="109" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="0">
+      <c r="B109">
         <v>108</v>
       </c>
     </row>
     <row r="110" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="0">
+      <c r="B110">
         <v>109</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="0">
+      <c r="B111">
         <v>110</v>
       </c>
     </row>
     <row r="112" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="0">
+      <c r="B112">
         <v>111</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="0">
+      <c r="B113">
         <v>112</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="0">
+      <c r="B114">
         <v>113</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="0">
+      <c r="B115">
         <v>114</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B116" s="0">
+      <c r="B116">
         <v>115</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="0">
+      <c r="B117">
         <v>116</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="0">
+      <c r="B118">
         <v>117</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B119" s="0">
+      <c r="B119">
         <v>118</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="0">
+      <c r="B120">
         <v>119</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="0">
+      <c r="B121">
         <v>120</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="0">
+      <c r="B122">
         <v>121</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="0">
+      <c r="B123">
         <v>122</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B124" s="0">
+      <c r="B124">
         <v>123</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="0">
+      <c r="B125">
         <v>124</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="0">
+      <c r="B126">
         <v>125</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="0">
+      <c r="B127">
         <v>126</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="0">
+      <c r="B128">
         <v>127</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="0">
+      <c r="B129">
         <v>128</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B130" s="0">
+      <c r="B130">
         <v>129</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="0">
+      <c r="B131">
         <v>130</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="0">
+      <c r="B132">
         <v>131</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="0">
+      <c r="B133">
         <v>132</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B134" s="0">
+      <c r="B134">
         <v>133</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B135" s="0">
+      <c r="B135">
         <v>134</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="0">
+      <c r="B136">
         <v>135</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B137" s="0">
+      <c r="B137">
         <v>136</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="0">
+      <c r="B138">
         <v>137</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="0">
+      <c r="B139">
         <v>138</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="0">
+      <c r="B140">
         <v>139</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B141" s="0">
+      <c r="B141">
         <v>140</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="0">
+      <c r="B142">
         <v>141</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="0">
+      <c r="B143">
         <v>142</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B144" s="0">
+      <c r="B144">
         <v>143</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="0">
+      <c r="B145">
         <v>144</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B146" s="0">
+      <c r="B146">
         <v>145</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B147" s="0">
+      <c r="B147">
         <v>146</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B148" s="0">
+      <c r="B148">
         <v>147</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="0">
+      <c r="B149">
         <v>148</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B150" s="0">
+      <c r="B150">
         <v>149</v>
       </c>
     </row>
     <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="0">
+      <c r="B151">
         <v>150</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B152" s="0">
+      <c r="B152">
         <v>151</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B153" s="0">
+      <c r="B153">
         <v>152</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="0">
+      <c r="B154">
         <v>153</v>
       </c>
     </row>
     <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B155" s="0">
+      <c r="B155">
         <v>154</v>
       </c>
     </row>
     <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="0">
+      <c r="B156">
         <v>155</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="0">
+      <c r="B157">
         <v>156</v>
       </c>
     </row>
     <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B158" s="0">
+      <c r="B158">
         <v>157</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="0">
+      <c r="B159">
         <v>158</v>
       </c>
     </row>
     <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="0">
+      <c r="B160">
         <v>159</v>
       </c>
     </row>
     <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B161" s="0">
+      <c r="B161">
         <v>160</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B162" s="0">
+      <c r="B162">
         <v>161</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="0">
+      <c r="B163">
         <v>162</v>
       </c>
     </row>
     <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="0">
+      <c r="B164">
         <v>163</v>
       </c>
     </row>
     <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B165" s="0">
+      <c r="B165">
         <v>164</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B166" s="0">
+      <c r="B166">
         <v>165</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="0">
+      <c r="B167">
         <v>166</v>
       </c>
     </row>
     <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B168" s="0">
+      <c r="B168">
         <v>167</v>
       </c>
     </row>
     <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B169" s="0">
+      <c r="B169">
         <v>168</v>
       </c>
     </row>
     <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B170" s="0">
+      <c r="B170">
         <v>169</v>
       </c>
     </row>
     <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B171" s="0">
+      <c r="B171">
         <v>170</v>
       </c>
     </row>
     <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B172" s="0">
+      <c r="B172">
         <v>171</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B173" s="0">
+      <c r="B173">
         <v>172</v>
       </c>
     </row>
     <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B174" s="0">
+      <c r="B174">
         <v>173</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B175" s="0">
+      <c r="B175">
         <v>174</v>
       </c>
     </row>
     <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B176" s="0">
+      <c r="B176">
         <v>175</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B177" s="0">
+      <c r="B177">
         <v>176</v>
       </c>
     </row>
     <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B178" s="0">
+      <c r="B178">
         <v>177</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B179" s="0">
+      <c r="B179">
         <v>178</v>
       </c>
     </row>
     <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B180" s="0">
+      <c r="B180">
         <v>179</v>
       </c>
     </row>
     <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B181" s="0">
+      <c r="B181">
         <v>180</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B182" s="0">
+      <c r="B182">
         <v>181</v>
       </c>
     </row>
     <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B183" s="0">
+      <c r="B183">
         <v>182</v>
       </c>
     </row>
     <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="0">
+      <c r="B184">
         <v>183</v>
       </c>
     </row>
     <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B185" s="0">
+      <c r="B185">
         <v>184</v>
       </c>
     </row>
     <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B186" s="0">
+      <c r="B186">
         <v>185</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B187" s="0">
+      <c r="B187">
         <v>186</v>
       </c>
     </row>
     <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="0">
+      <c r="B188">
         <v>187</v>
       </c>
     </row>
     <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="0">
+      <c r="B189">
         <v>188</v>
       </c>
     </row>
     <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B190" s="0">
+      <c r="B190">
         <v>189</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B191" s="0">
+      <c r="B191">
         <v>190</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B192" s="0">
+      <c r="B192">
         <v>191</v>
       </c>
     </row>
     <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B193" s="0">
+      <c r="B193">
         <v>192</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B194" s="0">
+      <c r="B194">
         <v>193</v>
       </c>
     </row>
     <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B195" s="0">
+      <c r="B195">
         <v>194</v>
       </c>
     </row>
     <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B196" s="0">
+      <c r="B196">
         <v>195</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B197" s="0">
+      <c r="B197">
         <v>196</v>
       </c>
     </row>
     <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="0">
+      <c r="B198">
         <v>197</v>
       </c>
     </row>
     <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B199" s="0">
+      <c r="B199">
         <v>198</v>
       </c>
     </row>
     <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B200" s="0">
+      <c r="B200">
         <v>199</v>
       </c>
     </row>
     <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B201" s="0">
+      <c r="B201">
         <v>200</v>
       </c>
     </row>
     <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B202" s="0">
+      <c r="B202">
         <v>201</v>
       </c>
     </row>
     <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B203" s="0">
+      <c r="B203">
         <v>202</v>
       </c>
     </row>
     <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B204" s="0">
+      <c r="B204">
         <v>203</v>
       </c>
     </row>
     <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B205" s="0">
+      <c r="B205">
         <v>204</v>
       </c>
     </row>
     <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B206" s="0">
+      <c r="B206">
         <v>205</v>
       </c>
     </row>
     <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B207" s="0">
+      <c r="B207">
         <v>206</v>
       </c>
     </row>
     <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B208" s="0">
+      <c r="B208">
         <v>207</v>
       </c>
     </row>
     <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B209" s="0">
+      <c r="B209">
         <v>208</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B210" s="0">
+      <c r="B210">
         <v>209</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B211" s="0">
+      <c r="B211">
         <v>210</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B212" s="0">
+      <c r="B212">
         <v>211</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B213" s="0">
+      <c r="B213">
         <v>212</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B214" s="0">
+      <c r="B214">
         <v>213</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B215" s="0">
+      <c r="B215">
         <v>214</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="0">
+      <c r="B216">
         <v>215</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="0">
+      <c r="B217">
         <v>216</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B218" s="0">
+      <c r="B218">
         <v>217</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="0">
+      <c r="B219">
         <v>218</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B220" s="0">
+      <c r="B220">
         <v>219</v>
       </c>
     </row>
     <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="0">
+      <c r="B221">
         <v>220</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B222" s="0">
+      <c r="B222">
         <v>221</v>
       </c>
     </row>
     <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="0">
+      <c r="B223">
         <v>222</v>
       </c>
     </row>
     <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="0">
+      <c r="B224">
         <v>223</v>
       </c>
     </row>
     <row r="225" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="0">
+      <c r="B225">
         <v>224</v>
       </c>
     </row>
     <row r="226" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B226" s="0">
+      <c r="B226">
         <v>225</v>
       </c>
     </row>
     <row r="227" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B227" s="0">
+      <c r="B227">
         <v>226</v>
       </c>
     </row>
     <row r="228" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="0">
+      <c r="B228">
         <v>227</v>
       </c>
     </row>
     <row r="229" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="0">
+      <c r="B229">
         <v>228</v>
       </c>
     </row>
     <row r="230" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B230" s="0">
+      <c r="B230">
         <v>229</v>
       </c>
     </row>
     <row r="231" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B231" s="0">
+      <c r="B231">
         <v>230</v>
       </c>
     </row>
     <row r="232" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B232" s="0">
+      <c r="B232">
         <v>231</v>
       </c>
     </row>
     <row r="233" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="0">
+      <c r="B233">
         <v>232</v>
       </c>
     </row>
     <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B234" s="0">
+      <c r="B234">
         <v>233</v>
       </c>
     </row>
     <row r="235" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B235" s="0">
+      <c r="B235">
         <v>234</v>
       </c>
     </row>
     <row r="236" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B236" s="0">
+      <c r="B236">
         <v>235</v>
       </c>
     </row>
     <row r="237" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="0">
+      <c r="B237">
         <v>236</v>
       </c>
     </row>
     <row r="238" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="0">
+      <c r="B238">
         <v>237</v>
       </c>
     </row>
     <row r="239" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="0">
+      <c r="B239">
         <v>238</v>
       </c>
     </row>
     <row r="240" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B240" s="0">
+      <c r="B240">
         <v>239</v>
       </c>
     </row>
     <row r="241" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="0">
+      <c r="B241">
         <v>240</v>
       </c>
     </row>
     <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="0">
+      <c r="B242">
         <v>241</v>
       </c>
     </row>
     <row r="243" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="0">
+      <c r="B243">
         <v>242</v>
       </c>
     </row>
     <row r="244" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="0">
+      <c r="B244">
         <v>243</v>
       </c>
     </row>
     <row r="245" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="0">
+      <c r="B245">
         <v>244</v>
       </c>
     </row>
     <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="0">
+      <c r="B246">
         <v>245</v>
       </c>
     </row>
     <row r="247" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="0">
+      <c r="B247">
         <v>246</v>
       </c>
     </row>
     <row r="248" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="0">
+      <c r="B248">
         <v>247</v>
       </c>
     </row>
     <row r="249" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="0">
+      <c r="B249">
         <v>248</v>
       </c>
     </row>
     <row r="250" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="0">
+      <c r="B250">
         <v>249</v>
       </c>
     </row>
     <row r="251" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="0">
+      <c r="B251">
         <v>250</v>
       </c>
     </row>
     <row r="252" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B252" s="0">
+      <c r="B252">
         <v>251</v>
       </c>
     </row>
     <row r="253" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="0">
+      <c r="B253">
         <v>252</v>
       </c>
     </row>
     <row r="254" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="0">
+      <c r="B254">
         <v>253</v>
       </c>
     </row>
     <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B255" s="0">
+      <c r="B255">
         <v>254</v>
       </c>
     </row>
     <row r="256" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B256" s="0">
+      <c r="B256">
         <v>255</v>
       </c>
     </row>
     <row r="257" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="0">
+      <c r="B257">
         <v>256</v>
       </c>
     </row>
     <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="0">
+      <c r="B258">
         <v>257</v>
       </c>
     </row>
     <row r="259" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="0">
+      <c r="B259">
         <v>258</v>
       </c>
     </row>
     <row r="260" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="0">
+      <c r="B260">
         <v>259</v>
       </c>
     </row>
     <row r="261" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="0">
+      <c r="B261">
         <v>260</v>
       </c>
     </row>
     <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="0">
+      <c r="B262">
         <v>261</v>
       </c>
     </row>
     <row r="263" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="0">
+      <c r="B263">
         <v>262</v>
       </c>
     </row>
     <row r="264" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="0">
+      <c r="B264">
         <v>263</v>
       </c>
     </row>
     <row r="265" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="0">
+      <c r="B265">
         <v>264</v>
       </c>
     </row>
     <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="0">
+      <c r="B266">
         <v>265</v>
       </c>
     </row>
     <row r="267" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B267" s="0">
+      <c r="B267">
         <v>266</v>
       </c>
     </row>
     <row r="268" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B268" s="0">
+      <c r="B268">
         <v>267</v>
       </c>
     </row>
     <row r="269" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B269" s="0">
+      <c r="B269">
         <v>268</v>
       </c>
     </row>
     <row r="270" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B270" s="0">
+      <c r="B270">
         <v>269</v>
       </c>
     </row>
     <row r="271" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="0">
+      <c r="B271">
         <v>270</v>
       </c>
     </row>
     <row r="272" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="0">
+      <c r="B272">
         <v>271</v>
       </c>
     </row>
     <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="0">
+      <c r="B273">
         <v>272</v>
       </c>
     </row>
     <row r="274" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="0">
+      <c r="B274">
         <v>273</v>
       </c>
     </row>
     <row r="275" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="0">
+      <c r="B275">
         <v>274</v>
       </c>
     </row>
     <row r="276" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="0">
+      <c r="B276">
         <v>275</v>
       </c>
     </row>
     <row r="277" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B277" s="0">
+      <c r="B277">
         <v>276</v>
       </c>
     </row>
     <row r="278" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B278" s="0">
+      <c r="B278">
         <v>277</v>
       </c>
     </row>
     <row r="279" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="0">
+      <c r="B279">
         <v>278</v>
       </c>
     </row>
     <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="0">
+      <c r="B280">
         <v>279</v>
       </c>
     </row>
     <row r="281" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B281" s="0">
+      <c r="B281">
         <v>280</v>
       </c>
     </row>
     <row r="282" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B282" s="0">
+      <c r="B282">
         <v>281</v>
       </c>
     </row>
     <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="0">
+      <c r="B283">
         <v>282</v>
       </c>
     </row>
     <row r="284" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="0">
+      <c r="B284">
         <v>283</v>
       </c>
     </row>
     <row r="285" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B285" s="0">
+      <c r="B285">
         <v>284</v>
       </c>
     </row>
     <row r="286" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="0">
+      <c r="B286">
         <v>285</v>
       </c>
     </row>
     <row r="287" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="0">
+      <c r="B287">
         <v>286</v>
       </c>
     </row>
     <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="0">
+      <c r="B288">
         <v>287</v>
       </c>
     </row>
     <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="0">
+      <c r="B289">
         <v>288</v>
       </c>
     </row>
     <row r="290" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B290" s="0">
+      <c r="B290">
         <v>289</v>
       </c>
     </row>
     <row r="291" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B291" s="0">
+      <c r="B291">
         <v>290</v>
       </c>
     </row>
     <row r="292" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B292" s="0">
+      <c r="B292">
         <v>291</v>
       </c>
     </row>
     <row r="293" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B293" s="0">
+      <c r="B293">
         <v>292</v>
       </c>
     </row>
     <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B294" s="0">
+      <c r="B294">
         <v>293</v>
       </c>
     </row>
     <row r="295" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B295" s="0">
+      <c r="B295">
         <v>294</v>
       </c>
     </row>
     <row r="296" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B296" s="0">
+      <c r="B296">
         <v>295</v>
       </c>
     </row>
     <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B297" s="0">
+      <c r="B297">
         <v>296</v>
       </c>
     </row>
     <row r="298" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="0">
+      <c r="B298">
         <v>297</v>
       </c>
     </row>
     <row r="299" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B299" s="0">
+      <c r="B299">
         <v>298</v>
       </c>
     </row>
     <row r="300" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B300" s="0">
+      <c r="B300">
         <v>299</v>
       </c>
     </row>
     <row r="301" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B301" s="0">
+      <c r="B301">
         <v>300</v>
       </c>
     </row>
     <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B302" s="0">
+      <c r="B302">
         <v>301</v>
       </c>
     </row>
     <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B303" s="0">
+      <c r="B303">
         <v>302</v>
       </c>
     </row>
     <row r="304" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B304" s="0">
+      <c r="B304">
         <v>303</v>
       </c>
     </row>
     <row r="305" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B305" s="0">
+      <c r="B305">
         <v>304</v>
       </c>
     </row>
     <row r="306" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B306" s="0">
+      <c r="B306">
         <v>305</v>
       </c>
     </row>
     <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B307" s="0">
+      <c r="B307">
         <v>306</v>
       </c>
     </row>
     <row r="308" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B308" s="0">
+      <c r="B308">
         <v>307</v>
       </c>
     </row>
     <row r="309" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B309" s="0">
+      <c r="B309">
         <v>308</v>
       </c>
     </row>
     <row r="310" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B310" s="0">
+      <c r="B310">
         <v>309</v>
       </c>
     </row>
     <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B311" s="0">
+      <c r="B311">
         <v>310</v>
       </c>
     </row>
     <row r="312" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B312" s="0">
+      <c r="B312">
         <v>311</v>
       </c>
     </row>
     <row r="313" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B313" s="0">
+      <c r="B313">
         <v>312</v>
       </c>
     </row>
     <row r="314" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B314" s="0">
+      <c r="B314">
         <v>313</v>
       </c>
     </row>
     <row r="315" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B315" s="0">
+      <c r="B315">
         <v>314</v>
       </c>
     </row>
     <row r="316" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B316" s="0">
+      <c r="B316">
         <v>315</v>
       </c>
     </row>
     <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B317" s="0">
+      <c r="B317">
         <v>316</v>
       </c>
     </row>
     <row r="318" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B318" s="0">
+      <c r="B318">
         <v>317</v>
       </c>
     </row>
     <row r="319" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B319" s="0">
+      <c r="B319">
         <v>318</v>
       </c>
     </row>
     <row r="320" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B320" s="0">
+      <c r="B320">
         <v>319</v>
       </c>
     </row>
     <row r="321" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B321" s="0">
+      <c r="B321">
         <v>320</v>
       </c>
     </row>
     <row r="322" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B322" s="0">
+      <c r="B322">
         <v>321</v>
       </c>
     </row>
     <row r="323" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B323" s="0">
+      <c r="B323">
         <v>322</v>
       </c>
     </row>
     <row r="324" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B324" s="0">
+      <c r="B324">
         <v>323</v>
       </c>
     </row>
     <row r="325" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B325" s="0">
+      <c r="B325">
         <v>324</v>
       </c>
     </row>
     <row r="326" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B326" s="0">
+      <c r="B326">
         <v>325</v>
       </c>
     </row>
     <row r="327" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B327" s="0">
+      <c r="B327">
         <v>326</v>
       </c>
     </row>
     <row r="328" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B328" s="0">
+      <c r="B328">
         <v>327</v>
       </c>
     </row>
     <row r="329" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B329" s="0">
+      <c r="B329">
         <v>328</v>
       </c>
     </row>
     <row r="330" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B330" s="0">
+      <c r="B330">
         <v>329</v>
       </c>
     </row>
     <row r="331" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B331" s="0">
+      <c r="B331">
         <v>330</v>
       </c>
     </row>
     <row r="332" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B332" s="0">
+      <c r="B332">
         <v>331</v>
       </c>
     </row>
     <row r="333" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B333" s="0">
+      <c r="B333">
         <v>332</v>
       </c>
     </row>
     <row r="334" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B334" s="0">
+      <c r="B334">
         <v>333</v>
       </c>
     </row>
     <row r="335" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B335" s="0">
+      <c r="B335">
         <v>334</v>
       </c>
     </row>
     <row r="336" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B336" s="0">
+      <c r="B336">
         <v>335</v>
       </c>
     </row>
     <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B337" s="0">
+      <c r="B337">
         <v>336</v>
       </c>
     </row>
     <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B338" s="0">
+      <c r="B338">
         <v>337</v>
       </c>
     </row>
     <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B339" s="0">
+      <c r="B339">
         <v>338</v>
       </c>
     </row>
     <row r="340" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B340" s="0">
+      <c r="B340">
         <v>339</v>
       </c>
     </row>
     <row r="341" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B341" s="0">
+      <c r="B341">
         <v>340</v>
       </c>
     </row>
     <row r="342" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B342" s="0">
+      <c r="B342">
         <v>341</v>
       </c>
     </row>
     <row r="343" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B343" s="0">
+      <c r="B343">
         <v>342</v>
       </c>
     </row>
     <row r="344" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B344" s="0">
+      <c r="B344">
         <v>343</v>
       </c>
     </row>
     <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B345" s="0">
+      <c r="B345">
         <v>344</v>
       </c>
     </row>
     <row r="346" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B346" s="0">
+      <c r="B346">
         <v>345</v>
       </c>
     </row>
     <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B347" s="0">
+      <c r="B347">
         <v>346</v>
       </c>
     </row>
     <row r="348" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B348" s="0">
+      <c r="B348">
         <v>347</v>
       </c>
     </row>
     <row r="349" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B349" s="0">
+      <c r="B349">
         <v>348</v>
       </c>
     </row>
     <row r="350" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B350" s="0">
+      <c r="B350">
         <v>349</v>
       </c>
     </row>
     <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B351" s="0">
+      <c r="B351">
         <v>350</v>
       </c>
     </row>
     <row r="352" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B352" s="0">
+      <c r="B352">
         <v>351</v>
       </c>
     </row>
     <row r="353" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B353" s="0">
+      <c r="B353">
         <v>352</v>
       </c>
     </row>
     <row r="354" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B354" s="0">
+      <c r="B354">
         <v>353</v>
       </c>
     </row>
     <row r="355" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B355" s="0">
+      <c r="B355">
         <v>354</v>
       </c>
     </row>
     <row r="356" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B356" s="0">
+      <c r="B356">
         <v>355</v>
       </c>
     </row>
     <row r="357" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B357" s="0">
+      <c r="B357">
         <v>356</v>
       </c>
     </row>
     <row r="358" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B358" s="0">
+      <c r="B358">
         <v>357</v>
       </c>
     </row>
     <row r="359" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B359" s="0">
+      <c r="B359">
         <v>358</v>
       </c>
     </row>
     <row r="360" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B360" s="0">
+      <c r="B360">
         <v>359</v>
       </c>
     </row>
     <row r="361" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B361" s="0">
+      <c r="B361">
         <v>360</v>
       </c>
     </row>
     <row r="362" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B362" s="0">
+      <c r="B362">
         <v>361</v>
       </c>
     </row>
     <row r="363" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B363" s="0">
+      <c r="B363">
         <v>362</v>
       </c>
     </row>
     <row r="364" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B364" s="0">
+      <c r="B364">
         <v>363</v>
       </c>
     </row>
     <row r="365" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B365" s="0">
+      <c r="B365">
         <v>364</v>
       </c>
     </row>
     <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B366" s="0">
+      <c r="B366">
         <v>365</v>
       </c>
     </row>
     <row r="367" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B367" s="0">
+      <c r="B367">
         <v>366</v>
       </c>
     </row>
     <row r="368" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B368" s="0">
+      <c r="B368">
         <v>367</v>
       </c>
     </row>
     <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B369" s="0">
+      <c r="B369">
         <v>368</v>
       </c>
     </row>
     <row r="370" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B370" s="0">
+      <c r="B370">
         <v>369</v>
       </c>
     </row>
     <row r="371" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B371" s="0">
+      <c r="B371">
         <v>370</v>
       </c>
     </row>
     <row r="372" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B372" s="0">
+      <c r="B372">
         <v>371</v>
       </c>
     </row>
     <row r="373" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B373" s="0">
+      <c r="B373">
         <v>372</v>
       </c>
     </row>
     <row r="374" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B374" s="0">
+      <c r="B374">
         <v>373</v>
       </c>
     </row>
     <row r="375" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B375" s="0">
+      <c r="B375">
         <v>374</v>
       </c>
     </row>
     <row r="376" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B376" s="0">
+      <c r="B376">
         <v>375</v>
       </c>
     </row>
     <row r="377" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B377" s="0">
+      <c r="B377">
         <v>376</v>
       </c>
     </row>
     <row r="378" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B378" s="0">
+      <c r="B378">
         <v>377</v>
       </c>
     </row>
     <row r="379" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B379" s="0">
+      <c r="B379">
         <v>378</v>
       </c>
     </row>
     <row r="380" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B380" s="0">
+      <c r="B380">
         <v>379</v>
       </c>
     </row>
     <row r="381" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B381" s="0">
+      <c r="B381">
         <v>380</v>
       </c>
     </row>
     <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B382" s="0">
+      <c r="B382">
         <v>381</v>
       </c>
     </row>
     <row r="383" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B383" s="0">
+      <c r="B383">
         <v>382</v>
       </c>
     </row>
     <row r="384" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B384" s="0">
+      <c r="B384">
         <v>383</v>
       </c>
     </row>
     <row r="385" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B385" s="0">
+      <c r="B385">
         <v>384</v>
       </c>
     </row>
     <row r="386" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B386" s="0">
+      <c r="B386">
         <v>385</v>
       </c>
     </row>
     <row r="387" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B387" s="0">
+      <c r="B387">
         <v>386</v>
       </c>
     </row>
     <row r="388" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B388" s="0">
+      <c r="B388">
         <v>387</v>
       </c>
     </row>
     <row r="389" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B389" s="0">
+      <c r="B389">
         <v>388</v>
       </c>
     </row>
     <row r="390" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B390" s="0">
+      <c r="B390">
         <v>389</v>
       </c>
     </row>
     <row r="391" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B391" s="0">
+      <c r="B391">
         <v>390</v>
       </c>
     </row>
     <row r="392" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B392" s="0">
+      <c r="B392">
         <v>391</v>
       </c>
     </row>
     <row r="393" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B393" s="0">
+      <c r="B393">
         <v>392</v>
       </c>
     </row>
     <row r="394" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B394" s="0">
+      <c r="B394">
         <v>393</v>
       </c>
     </row>
     <row r="395" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B395" s="0">
+      <c r="B395">
         <v>394</v>
       </c>
     </row>
     <row r="396" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B396" s="0">
+      <c r="B396">
         <v>395</v>
       </c>
     </row>
     <row r="397" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B397" s="0">
+      <c r="B397">
         <v>396</v>
       </c>
     </row>
     <row r="398" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B398" s="0">
+      <c r="B398">
         <v>397</v>
       </c>
     </row>
     <row r="399" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B399" s="0">
+      <c r="B399">
         <v>398</v>
       </c>
     </row>
     <row r="400" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B400" s="0">
+      <c r="B400">
         <v>399</v>
       </c>
     </row>
     <row r="401" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B401" s="0">
+      <c r="B401">
         <v>400</v>
       </c>
     </row>
     <row r="402" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B402" s="0">
+      <c r="B402">
         <v>401</v>
       </c>
     </row>
     <row r="403" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B403" s="0">
+      <c r="B403">
         <v>402</v>
       </c>
     </row>
     <row r="404" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B404" s="0">
+      <c r="B404">
         <v>403</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed IOException issue in Filewriter
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0002D2EA-846F-44D6-91C4-7756969E29DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A9C760-2678-4985-ACD2-7300FC0D713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,7 +314,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed time logic from GUI and forced all time references to go through ProjectTimer class
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A9C760-2678-4985-ACD2-7300FC0D713A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6109AA8-0A16-404F-B7C9-B6DD9419B00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,6 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -314,7 +315,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -347,22 +348,40 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
+      <c r="C2" t="n" s="0">
+        <v>5.264999866485596</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>3.0</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="0">
         <v>2</v>
       </c>
+      <c r="C3" t="n" s="0">
+        <v>0.8740000128746033</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>-1.0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="0">
         <v>3</v>
       </c>
+      <c r="C4" t="n" s="0">
+        <v>33.07899856567383</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="0">
         <v>4</v>
       </c>
     </row>
@@ -372,17 +391,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="B8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="B9" s="0">
         <v>8</v>
       </c>
     </row>
@@ -392,17 +411,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11">
+      <c r="B11" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12">
+      <c r="B12" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="0">
         <v>12</v>
       </c>
     </row>
@@ -412,17 +431,17 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17">
+      <c r="B17" s="0">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed getCutLengthMethod from GUI that was calculating the length locally. Moved all of that logic to the actuator class.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -384,15 +384,33 @@
       <c r="B5" s="0">
         <v>4</v>
       </c>
+      <c r="C5" t="n" s="0">
+        <v>8.196999549865723</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
+      <c r="C6" t="n" s="0">
+        <v>17.131999969482422</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="0">
         <v>6</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>5.175000190734863</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>60.0</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ListeningAdapter class to remove empty @Override methods from GUI. Empty methods now live in ListeningAdapter.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -417,10 +417,22 @@
       <c r="B8" s="0">
         <v>7</v>
       </c>
+      <c r="C8" t="n" s="0">
+        <v>4.9730000495910645</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="0">
         <v>8</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>1.8899999856948853</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>20.0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cleaned up some formatting, removed unused variables and added a few comments
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6109AA8-0A16-404F-B7C9-B6DD9419B00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BD4F4A-B60A-4B12-BF58-62875DCB1F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -315,7 +315,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -349,10 +349,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>5.264999866485596</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>3.0</v>
+        <v>2.263000011444092</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20.0</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>
@@ -362,77 +362,35 @@
       <c r="B3" s="0">
         <v>2</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>0.8740000128746033</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>-1.0</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="0">
         <v>3</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>33.07899856567383</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>20.0</v>
-      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="0">
         <v>4</v>
       </c>
-      <c r="C5" t="n" s="0">
-        <v>8.196999549865723</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>20.0</v>
-      </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" t="n" s="0">
-        <v>17.131999969482422</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>20.0</v>
-      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="0">
         <v>6</v>
       </c>
-      <c r="C7" t="n" s="0">
-        <v>5.175000190734863</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>60.0</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="0">
         <v>7</v>
       </c>
-      <c r="C8" t="n" s="0">
-        <v>4.9730000495910645</v>
-      </c>
-      <c r="D8" t="n" s="0">
-        <v>20.0</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="0">
         <v>8</v>
-      </c>
-      <c r="C9" t="n" s="0">
-        <v>1.8899999856948853</v>
-      </c>
-      <c r="D9" t="n" s="0">
-        <v>20.0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added first artifact and executable Jar file and confirmed it works from desktop! Will create another with icon in future.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -351,7 +351,7 @@
       <c r="C2" t="n" s="0">
         <v>2.263000011444092</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="n" s="0">
         <v>20.0</v>
       </c>
       <c r="E2" s="2"/>
@@ -362,15 +362,33 @@
       <c r="B3" s="0">
         <v>2</v>
       </c>
+      <c r="C3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="0">
         <v>3</v>
       </c>
+      <c r="C4" t="n" s="0">
+        <v>3.546999931335449</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="0">
         <v>4</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>3.421999931335449</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>51.0</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor refactoring. Created Clickable JAR.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,19 +3,32 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BD4F4A-B60A-4B12-BF58-62875DCB1F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C34440-F4B8-4461-B054-3621DD85EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -47,7 +60,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -315,7 +327,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -348,66 +360,84 @@
       <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="n" s="0">
-        <v>2.263000011444092</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>20.0</v>
+      <c r="C2">
+        <v>2.2630000114440918</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="F2" s="3">
+        <f>SUM(C2:C300)</f>
+        <v>17.881999969482422</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUM(D2:D300)</f>
+        <v>124</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="0">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>20.0</v>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="0">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" t="n" s="0">
-        <v>3.546999931335449</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>16.0</v>
+      <c r="C4">
+        <v>3.5469999313354492</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="0">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" t="n" s="0">
-        <v>3.421999931335449</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>51.0</v>
+      <c r="C5">
+        <v>3.4219999313354492</v>
+      </c>
+      <c r="D5">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>7.6500000953674316</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="0">
+      <c r="B7">
         <v>6</v>
       </c>
+      <c r="C7">
+        <v>2.5550000667572021</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="0">
+      <c r="B8">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="0">
+      <c r="B9">
         <v>8</v>
       </c>
     </row>
@@ -417,17 +447,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="0">
+      <c r="B11">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="0">
+      <c r="B12">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="0">
+      <c r="B13">
         <v>12</v>
       </c>
     </row>
@@ -437,17 +467,17 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="0">
+      <c r="B15">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="0">
+      <c r="B16">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="0">
+      <c r="B17">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed all non variable constants from GUI. Moved angle and position checking logic to respective classes. Confirmed as working.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C34440-F4B8-4461-B054-3621DD85EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB4F4E2-8D0E-4398-8214-4AFCC4D631B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Project Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Pieces</t>
   </si>
@@ -53,13 +50,14 @@
     <t>Total Material</t>
   </si>
   <si>
-    <t>Test Project!</t>
+    <t>PNAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -324,162 +322,98 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2.2630000114440918</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3">
-        <f>SUM(C2:C300)</f>
-        <v>17.881999969482422</v>
-      </c>
-      <c r="G2" s="3">
-        <f>SUM(D2:D300)</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3.5469999313354492</v>
-      </c>
-      <c r="D4">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>3.4219999313354492</v>
-      </c>
-      <c r="D5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>7.6500000953674316</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2.5550000667572021</v>
-      </c>
-      <c r="D7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>8</v>
+    </row>
+    <row r="2">
+      <c r="B2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="n" s="0">
+        <v>0.722000002861023</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>11.496000289916992</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="C4" t="n" s="0">
+        <v>12.045000076293945</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="C5" t="n" s="0">
+        <v>6.734000205993652</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="C6" t="n" s="0">
+        <v>3.4179999828338623</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>30.0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>12</v>
-      </c>
-    </row>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>16</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Refactoring, lots of comments added, removed a few unused methods / variables.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -406,6 +406,17 @@
         <v>30.0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="B7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>3.0350000858306885</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>140.0</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added Javadoc, Javadoc comments for all methods and Final UML Diagram.
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -417,6 +417,17 @@
         <v>140.0</v>
       </c>
     </row>
+    <row r="8">
+      <c r="B8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="C8" t="n" s="0">
+        <v>20.441999435424805</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>14.0</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
     </row>

</xml_diff>

<commit_message>
Added folder for and all .STL files of 3d Models
</commit_message>
<xml_diff>
--- a/Excel Sheets/Kumiko Example.xlsx
+++ b/Excel Sheets/Kumiko Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aklug\Desktop\Kumiko Project\KumikoMachine\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB4F4E2-8D0E-4398-8214-4AFCC4D631B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275A56C-8649-4492-B303-0BB3C0501EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>Total Material</t>
   </si>
   <si>
-    <t>PNAME</t>
+    <t>EXAMPLE PROJECT</t>
   </si>
 </sst>
 </file>
@@ -329,6 +329,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="19.77734375"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -351,81 +354,92 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="C2" t="n" s="0">
-        <v>0.722000002861023</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C3" t="n" s="0">
+    <row r="2" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0.72200000286102295</v>
+      </c>
+      <c r="D2" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0">
         <v>11.496000289916992</v>
       </c>
-      <c r="D3" t="n" s="0">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="n" s="0">
+      <c r="D3" s="0">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B4" s="0">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0">
+        <v>12.045000076293945</v>
+      </c>
+      <c r="D4" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B5" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0">
+        <v>6.7340002059936523</v>
+      </c>
+      <c r="D5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B6" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
+        <v>3.4179999828338623</v>
+      </c>
+      <c r="D6" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B7" s="0">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0">
+        <v>3.0350000858306885</v>
+      </c>
+      <c r="D7" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0">
+        <v>20.441999435424805</v>
+      </c>
+      <c r="D8" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>112.50800323486328</v>
+      </c>
+      <c r="D9" t="n" s="0">
         <v>3.0</v>
-      </c>
-      <c r="C4" t="n" s="0">
-        <v>12.045000076293945</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="C5" t="n" s="0">
-        <v>6.734000205993652</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="C6" t="n" s="0">
-        <v>3.4179999828338623</v>
-      </c>
-      <c r="D6" t="n" s="0">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="C7" t="n" s="0">
-        <v>3.0350000858306885</v>
-      </c>
-      <c r="D7" t="n" s="0">
-        <v>140.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="C8" t="n" s="0">
-        <v>20.441999435424805</v>
-      </c>
-      <c r="D8" t="n" s="0">
-        <v>14.0</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>